<commit_message>
Test case 13 completed, is successfully running
</commit_message>
<xml_diff>
--- a/RTuinOS/code/applications/tc13/testSequence.xlsx
+++ b/RTuinOS/code/applications/tc13/testSequence.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="29">
   <si>
     <t>Action</t>
   </si>
@@ -82,35 +82,42 @@
     <t>Step</t>
   </si>
   <si>
-    <t>Task T0C0 (Priority 0)</t>
-  </si>
-  <si>
-    <t>Task T0C1 (Priority 1)</t>
-  </si>
-  <si>
-    <t>Task T0C2 (Priority 2)</t>
-  </si>
-  <si>
     <t>Initial condition: Both semaphores start with 2</t>
   </si>
   <si>
-    <t>T0C0</t>
-  </si>
-  <si>
-    <t>T0C1</t>
-  </si>
-  <si>
-    <t>T0C2</t>
+    <t>Task T0 (Priority 0)</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>Task T1 (Priority 1)</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>Task T2 (Priority 2)</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -475,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -500,9 +507,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,37 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,7 +855,7 @@
   <dimension ref="A2:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,41 +865,41 @@
   <sheetData>
     <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="27" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="36" t="s">
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="37"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="39"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -900,43 +908,43 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="26" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="30"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="46"/>
       <c r="AA4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="46"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="42"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
@@ -1010,22 +1018,22 @@
       <c r="Y5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="31" t="s">
+      <c r="Z5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="AA5" s="43" t="s">
+      <c r="AA5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="AB5" s="48" t="s">
+      <c r="AB5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="AC5" s="44" t="s">
+      <c r="AC5" s="33" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -1065,23 +1073,23 @@
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="41">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="47">
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="34">
         <v>2</v>
       </c>
-      <c r="AC6" s="42">
+      <c r="AC6" s="31">
         <v>1</v>
       </c>
       <c r="AE6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -1131,14 +1139,14 @@
       <c r="W7" s="16"/>
       <c r="X7" s="16"/>
       <c r="Y7" s="16"/>
-      <c r="Z7" s="33"/>
+      <c r="Z7" s="26"/>
       <c r="AA7" s="3">
         <v>2</v>
       </c>
       <c r="AB7" s="1">
         <v>2</v>
       </c>
-      <c r="AC7" s="38">
+      <c r="AC7" s="28">
         <v>0</v>
       </c>
     </row>
@@ -1196,18 +1204,18 @@
         <v>13</v>
       </c>
       <c r="Y8" s="16"/>
-      <c r="Z8" s="33" t="s">
+      <c r="Z8" s="26" t="s">
         <v>13</v>
       </c>
       <c r="AA8" s="3">
         <v>3</v>
       </c>
       <c r="AB8" s="1"/>
-      <c r="AC8" s="38"/>
+      <c r="AC8" s="28"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -1253,7 +1261,7 @@
         <v>12</v>
       </c>
       <c r="Y9" s="16"/>
-      <c r="Z9" s="33">
+      <c r="Z9" s="26">
         <v>1</v>
       </c>
       <c r="AA9" s="3">
@@ -1262,13 +1270,13 @@
       <c r="AB9" s="1">
         <v>2</v>
       </c>
-      <c r="AC9" s="38">
+      <c r="AC9" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1310,7 +1318,7 @@
         <v>12</v>
       </c>
       <c r="Y10" s="16"/>
-      <c r="Z10" s="33">
+      <c r="Z10" s="26">
         <v>1</v>
       </c>
       <c r="AA10" s="3">
@@ -1319,13 +1327,13 @@
       <c r="AB10" s="1">
         <v>2</v>
       </c>
-      <c r="AC10" s="38">
+      <c r="AC10" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -1363,7 +1371,7 @@
         <v>12</v>
       </c>
       <c r="Y11" s="16"/>
-      <c r="Z11" s="33">
+      <c r="Z11" s="26">
         <v>1</v>
       </c>
       <c r="AA11" s="3">
@@ -1372,7 +1380,7 @@
       <c r="AB11" s="1">
         <v>2</v>
       </c>
-      <c r="AC11" s="38">
+      <c r="AC11" s="28">
         <v>0</v>
       </c>
     </row>
@@ -1422,7 +1430,7 @@
       <c r="Y12" s="16">
         <v>1</v>
       </c>
-      <c r="Z12" s="33">
+      <c r="Z12" s="26">
         <v>1</v>
       </c>
       <c r="AA12" s="3">
@@ -1431,13 +1439,13 @@
       <c r="AB12" s="1">
         <v>1</v>
       </c>
-      <c r="AC12" s="38">
+      <c r="AC12" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -1479,18 +1487,22 @@
       <c r="Y13" s="16">
         <v>1</v>
       </c>
-      <c r="Z13" s="33">
+      <c r="Z13" s="26">
         <v>1</v>
       </c>
       <c r="AA13" s="3">
         <v>8</v>
       </c>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="38"/>
+      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="28">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -1532,14 +1544,18 @@
       <c r="Y14" s="16">
         <v>1</v>
       </c>
-      <c r="Z14" s="33">
+      <c r="Z14" s="26">
         <v>1</v>
       </c>
       <c r="AA14" s="3">
         <v>9</v>
       </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="38"/>
+      <c r="AB14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="28">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1583,20 +1599,20 @@
       <c r="W15" s="16"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="16"/>
-      <c r="Z15" s="33"/>
+      <c r="Z15" s="26"/>
       <c r="AA15" s="3">
         <v>10</v>
       </c>
       <c r="AB15" s="1">
         <v>2</v>
       </c>
-      <c r="AC15" s="38">
+      <c r="AC15" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -1636,20 +1652,20 @@
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
       <c r="Y16" s="16"/>
-      <c r="Z16" s="33"/>
+      <c r="Z16" s="26"/>
       <c r="AA16" s="3">
         <v>11</v>
       </c>
       <c r="AB16" s="1">
         <v>1</v>
       </c>
-      <c r="AC16" s="38">
+      <c r="AC16" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>11</v>
@@ -1691,20 +1707,20 @@
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
       <c r="Y17" s="16"/>
-      <c r="Z17" s="33"/>
+      <c r="Z17" s="26"/>
       <c r="AA17" s="3">
         <v>12</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
       </c>
-      <c r="AC17" s="38">
+      <c r="AC17" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
@@ -1746,20 +1762,20 @@
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
       <c r="Y18" s="16"/>
-      <c r="Z18" s="33"/>
+      <c r="Z18" s="26"/>
       <c r="AA18" s="3">
         <v>13</v>
       </c>
       <c r="AB18" s="1">
         <v>0</v>
       </c>
-      <c r="AC18" s="38">
+      <c r="AC18" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
@@ -1783,8 +1799,8 @@
       <c r="M19" s="16">
         <v>3</v>
       </c>
-      <c r="N19" s="17" t="s">
-        <v>17</v>
+      <c r="N19" s="17">
+        <v>1</v>
       </c>
       <c r="O19" s="18"/>
       <c r="P19" s="16"/>
@@ -1799,14 +1815,14 @@
       <c r="W19" s="16"/>
       <c r="X19" s="16"/>
       <c r="Y19" s="16"/>
-      <c r="Z19" s="33"/>
+      <c r="Z19" s="26"/>
       <c r="AA19" s="3">
         <v>14</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
       </c>
-      <c r="AC19" s="38">
+      <c r="AC19" s="28">
         <v>0</v>
       </c>
       <c r="AE19" t="s">
@@ -1815,7 +1831,7 @@
     </row>
     <row r="20" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
@@ -1840,7 +1856,7 @@
         <v>3</v>
       </c>
       <c r="N20" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O20" s="18"/>
       <c r="P20" s="16"/>
@@ -1853,16 +1869,21 @@
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
       <c r="Y20" s="16"/>
-      <c r="Z20" s="33"/>
+      <c r="Z20" s="26"/>
       <c r="AA20" s="3">
         <v>15</v>
       </c>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="38"/>
+      <c r="AB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="28">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="36"/>
     </row>
     <row r="21" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
@@ -1886,9 +1907,7 @@
       <c r="M21" s="16">
         <v>2</v>
       </c>
-      <c r="N21" s="17">
-        <v>1</v>
-      </c>
+      <c r="N21" s="17"/>
       <c r="O21" s="18"/>
       <c r="P21" s="16"/>
       <c r="Q21" s="16"/>
@@ -1900,20 +1919,20 @@
       <c r="W21" s="16"/>
       <c r="X21" s="16"/>
       <c r="Y21" s="16"/>
-      <c r="Z21" s="33"/>
+      <c r="Z21" s="26"/>
       <c r="AA21" s="3">
         <v>16</v>
       </c>
       <c r="AB21" s="1">
         <v>1</v>
       </c>
-      <c r="AC21" s="38">
-        <v>1</v>
+      <c r="AC21" s="28">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1925,9 +1944,7 @@
       <c r="G22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="17" t="s">
-        <v>12</v>
-      </c>
+      <c r="H22" s="17"/>
       <c r="I22" s="18"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
@@ -1947,20 +1964,20 @@
       <c r="W22" s="16"/>
       <c r="X22" s="16"/>
       <c r="Y22" s="16"/>
-      <c r="Z22" s="33"/>
+      <c r="Z22" s="26"/>
       <c r="AA22" s="3">
         <v>17</v>
       </c>
       <c r="AB22" s="1">
         <v>2</v>
       </c>
-      <c r="AC22" s="38">
+      <c r="AC22" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -1990,14 +2007,14 @@
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
       <c r="Y23" s="16"/>
-      <c r="Z23" s="33"/>
+      <c r="Z23" s="26"/>
       <c r="AA23" s="3">
         <v>18</v>
       </c>
       <c r="AB23" s="1">
         <v>3</v>
       </c>
-      <c r="AC23" s="38">
+      <c r="AC23" s="28">
         <v>2</v>
       </c>
     </row>
@@ -2035,14 +2052,14 @@
       <c r="Y24" s="16">
         <v>1</v>
       </c>
-      <c r="Z24" s="33"/>
+      <c r="Z24" s="26"/>
       <c r="AA24" s="3">
         <v>19</v>
       </c>
       <c r="AB24" s="1">
         <v>2</v>
       </c>
-      <c r="AC24" s="38">
+      <c r="AC24" s="28">
         <v>2</v>
       </c>
       <c r="AE24" t="s">
@@ -2075,10 +2092,10 @@
       <c r="W25" s="20"/>
       <c r="X25" s="20"/>
       <c r="Y25" s="20"/>
-      <c r="Z25" s="34"/>
+      <c r="Z25" s="27"/>
       <c r="AA25" s="4"/>
       <c r="AB25" s="6"/>
-      <c r="AC25" s="39"/>
+      <c r="AC25" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2092,5 +2109,6 @@
     <mergeCell ref="I3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>